<commit_message>
mis-tareas: cambios de estado en el canvan incluye: derivaciones, asignaciones y delegaciones
</commit_message>
<xml_diff>
--- a/docs/KanVan.xlsx
+++ b/docs/KanVan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpleitez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gestor-de-tareas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C44034C1-1B93-49A5-A005-3913A08CC57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E20BFAD-4BC0-415E-BD94-123D8B12E832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30AB5270-AFA5-4EE9-9E71-0F47B3D76406}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Recepciones</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Pasos</t>
   </si>
   <si>
-    <t>Atenciones</t>
-  </si>
-  <si>
     <t>Recepcion</t>
   </si>
   <si>
@@ -81,13 +75,67 @@
   </si>
   <si>
     <t>INTEGRACION DE KANVAN A LA ESTRUCTURA DEL SISTEMA</t>
+  </si>
+  <si>
+    <t>Atencion</t>
+  </si>
+  <si>
+    <t>Accion</t>
+  </si>
+  <si>
+    <t>Derivar</t>
+  </si>
+  <si>
+    <t>Asignar</t>
+  </si>
+  <si>
+    <t>Delegar</t>
+  </si>
+  <si>
+    <t>Procesar</t>
+  </si>
+  <si>
+    <t>Entregar</t>
+  </si>
+  <si>
+    <t>Areas</t>
+  </si>
+  <si>
+    <t>Destino</t>
+  </si>
+  <si>
+    <t>Distrito y oficina</t>
+  </si>
+  <si>
+    <t>Beneficiario</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Solicitud</t>
+  </si>
+  <si>
+    <t>Equipos</t>
+  </si>
+  <si>
+    <t>Operadores</t>
+  </si>
+  <si>
+    <t>Beneficiarios</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Enviar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +150,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -112,30 +166,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -143,6 +173,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9933"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -159,25 +213,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -186,6 +257,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9933"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -514,99 +593,167 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{130AF9D9-ADD9-43A5-ADD2-8859ECE83241}">
-  <dimension ref="B3:G9"/>
+  <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2025000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2025000001</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2025000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2025000001</v>
+      </c>
+      <c r="H7" s="3">
+        <v>2025000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2025000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2025000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2025000003</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2025000004</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2025000005</v>
+      </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>2025000001</v>
-      </c>
-      <c r="D9">
-        <v>2025000002</v>
-      </c>
-      <c r="E9">
-        <v>2025000003</v>
-      </c>
-      <c r="F9">
-        <v>2025000004</v>
-      </c>
-      <c r="G9">
-        <v>2025000005</v>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>